<commit_message>
week 10 sum 2022 updates
</commit_message>
<xml_diff>
--- a/data/InningCounts.xlsx
+++ b/data/InningCounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED82A61-FAD1-442A-8090-216035BA7410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12D2118-E3BD-44B1-8796-907313D9877D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20955" yWindow="1860" windowWidth="15150" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19140" yWindow="0" windowWidth="15150" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Player</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Week 27</t>
+  </si>
+  <si>
+    <t>Week 28</t>
   </si>
 </sst>
 </file>
@@ -476,11 +479,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB9"/>
+  <dimension ref="A1:AC9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L15" sqref="L15"/>
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,7 +495,7 @@
     <col min="21" max="21" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +580,11 @@
       <c r="AB1" t="s">
         <v>35</v>
       </c>
+      <c r="AC1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -643,7 +649,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -684,7 +690,7 @@
         <v>4.67</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -706,8 +712,11 @@
       <c r="AA4">
         <v>7</v>
       </c>
+      <c r="AC4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -751,7 +760,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -803,8 +812,11 @@
       <c r="AB6">
         <v>10</v>
       </c>
+      <c r="AC6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -850,8 +862,11 @@
       <c r="AB7">
         <v>6.5</v>
       </c>
+      <c r="AC7">
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -900,8 +915,11 @@
       <c r="AA8">
         <v>3.67</v>
       </c>
+      <c r="AC8">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -921,6 +939,9 @@
         <v>1.5</v>
       </c>
       <c r="AB9">
+        <v>1.5</v>
+      </c>
+      <c r="AC9">
         <v>1.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
summer week 11 inputs
</commit_message>
<xml_diff>
--- a/data/InningCounts.xlsx
+++ b/data/InningCounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12D2118-E3BD-44B1-8796-907313D9877D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD50F11-277A-4D6F-9E8A-855EA24024C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19140" yWindow="0" windowWidth="15150" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3645" yWindow="2625" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Player</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Week 28</t>
+  </si>
+  <si>
+    <t>Week 29</t>
   </si>
 </sst>
 </file>
@@ -479,11 +482,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC9"/>
+  <dimension ref="A1:AD9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD12" sqref="AD12"/>
+      <selection pane="topRight" activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +498,7 @@
     <col min="21" max="21" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -583,8 +586,11 @@
       <c r="AC1" t="s">
         <v>36</v>
       </c>
+      <c r="AD1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -648,8 +654,11 @@
       <c r="AB2">
         <v>3.5</v>
       </c>
+      <c r="AD2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -690,7 +699,7 @@
         <v>4.67</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -715,8 +724,11 @@
       <c r="AC4">
         <v>7</v>
       </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -760,7 +772,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -815,8 +827,11 @@
       <c r="AC6">
         <v>7</v>
       </c>
+      <c r="AD6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -866,7 +881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -918,8 +933,11 @@
       <c r="AC8">
         <v>3.5</v>
       </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -943,6 +961,9 @@
       </c>
       <c r="AC9">
         <v>1.5</v>
+      </c>
+      <c r="AD9">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sum 22 week 13 innings
</commit_message>
<xml_diff>
--- a/data/InningCounts.xlsx
+++ b/data/InningCounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD50F11-277A-4D6F-9E8A-855EA24024C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D7181D-A4A8-4713-9667-8A7898FB6FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="2625" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="3390" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Player</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Week 29</t>
+  </si>
+  <si>
+    <t>Week 30</t>
   </si>
 </sst>
 </file>
@@ -482,11 +485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD9"/>
+  <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE6" sqref="AE6"/>
+      <selection pane="topRight" activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +501,7 @@
     <col min="21" max="21" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,8 +592,11 @@
       <c r="AD1" t="s">
         <v>37</v>
       </c>
+      <c r="AE1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -657,8 +663,11 @@
       <c r="AD2">
         <v>4</v>
       </c>
+      <c r="AE2">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -698,8 +707,11 @@
       <c r="AB3">
         <v>4.67</v>
       </c>
+      <c r="AE3">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -727,8 +739,11 @@
       <c r="AD4">
         <v>0</v>
       </c>
+      <c r="AE4">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -771,8 +786,11 @@
       <c r="Z5">
         <v>5.5</v>
       </c>
+      <c r="AE5">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -831,7 +849,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -881,7 +899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -937,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -964,6 +982,9 @@
       </c>
       <c r="AD9">
         <v>2.5</v>
+      </c>
+      <c r="AE9">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
week 14 sum 22 recorded
</commit_message>
<xml_diff>
--- a/data/InningCounts.xlsx
+++ b/data/InningCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D7181D-A4A8-4713-9667-8A7898FB6FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5EF81E-7F2A-4D71-BE13-12C1682E3953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="3390" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Player</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Week 30</t>
+  </si>
+  <si>
+    <t>Week 31</t>
   </si>
 </sst>
 </file>
@@ -485,11 +488,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE9"/>
+  <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z14" sqref="Z14"/>
+      <selection pane="topRight" activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +504,7 @@
     <col min="21" max="21" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -595,8 +598,11 @@
       <c r="AE1" t="s">
         <v>38</v>
       </c>
+      <c r="AF1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -667,7 +673,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -710,8 +716,11 @@
       <c r="AE3">
         <v>2.5</v>
       </c>
+      <c r="AF3">
+        <v>2.75</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -743,7 +752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -789,8 +798,11 @@
       <c r="AE5">
         <v>10</v>
       </c>
+      <c r="AF5">
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -848,8 +860,11 @@
       <c r="AD6">
         <v>10</v>
       </c>
+      <c r="AF6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -898,8 +913,11 @@
       <c r="AC7">
         <v>5</v>
       </c>
+      <c r="AF7">
+        <v>7</v>
+      </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -954,8 +972,11 @@
       <c r="AD8">
         <v>0</v>
       </c>
+      <c r="AF8">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
week 15 sum 22 innings recorded
</commit_message>
<xml_diff>
--- a/data/InningCounts.xlsx
+++ b/data/InningCounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5EF81E-7F2A-4D71-BE13-12C1682E3953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD561FAA-E81A-4432-A3EE-68B2E4721BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="3390" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4065" yWindow="705" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Player</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Week 31</t>
+  </si>
+  <si>
+    <t>Week 32</t>
   </si>
 </sst>
 </file>
@@ -488,11 +491,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:AG9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE14" sqref="AE14"/>
+      <selection pane="topRight" activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +507,7 @@
     <col min="21" max="21" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,8 +604,11 @@
       <c r="AF1" t="s">
         <v>39</v>
       </c>
+      <c r="AG1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -672,8 +678,11 @@
       <c r="AE2">
         <v>3.5</v>
       </c>
+      <c r="AG2">
+        <v>1.75</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -720,7 +729,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -751,8 +760,11 @@
       <c r="AE4">
         <v>7</v>
       </c>
+      <c r="AG4">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -801,8 +813,11 @@
       <c r="AF5">
         <v>7</v>
       </c>
+      <c r="AG5">
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -863,8 +878,11 @@
       <c r="AF6">
         <v>7</v>
       </c>
+      <c r="AG6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -917,7 +935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -976,7 +994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1006,6 +1024,9 @@
       </c>
       <c r="AE9">
         <v>1.5</v>
+      </c>
+      <c r="AG9">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed inning averages under 20 matches
</commit_message>
<xml_diff>
--- a/data/InningCounts.xlsx
+++ b/data/InningCounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA91268C-B344-436B-A6CF-9C3F6F5E502A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA44764-2E71-41E4-BA10-500795AA8DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4065" yWindow="705" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,8 +494,8 @@
   <dimension ref="A1:AG9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AG11" sqref="AG11"/>
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
summer 2022 week 16 innings
</commit_message>
<xml_diff>
--- a/data/InningCounts.xlsx
+++ b/data/InningCounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA44764-2E71-41E4-BA10-500795AA8DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5886945-CFE2-4842-B511-1BE917C76651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="705" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20610" yWindow="1995" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Player</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Week 32</t>
+  </si>
+  <si>
+    <t>Week 33</t>
   </si>
 </sst>
 </file>
@@ -491,11 +494,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z16" sqref="Z16"/>
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +510,7 @@
     <col min="21" max="21" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,8 +610,11 @@
       <c r="AG1" t="s">
         <v>40</v>
       </c>
+      <c r="AH1" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -682,7 +688,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -728,8 +734,11 @@
       <c r="AF3">
         <v>2.75</v>
       </c>
+      <c r="AH3">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -764,7 +773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -817,7 +826,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -881,8 +890,11 @@
       <c r="AG6">
         <v>5</v>
       </c>
+      <c r="AH6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -934,8 +946,11 @@
       <c r="AF7">
         <v>5.5</v>
       </c>
+      <c r="AH7">
+        <v>9</v>
+      </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -993,8 +1008,11 @@
       <c r="AF8">
         <v>2</v>
       </c>
+      <c r="AH8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1027,6 +1045,9 @@
       </c>
       <c r="AG9">
         <v>10</v>
+      </c>
+      <c r="AH9">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
week 3 inn inputs week 2 results inputs
</commit_message>
<xml_diff>
--- a/data/InningCounts.xlsx
+++ b/data/InningCounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5886945-CFE2-4842-B511-1BE917C76651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B87F4A-B27F-4186-9ED7-B9B0CC464D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20610" yWindow="1995" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20865" yWindow="1425" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Player</t>
   </si>
@@ -161,6 +161,24 @@
   </si>
   <si>
     <t>Week 33</t>
+  </si>
+  <si>
+    <t>Week 34</t>
+  </si>
+  <si>
+    <t>Week 35</t>
+  </si>
+  <si>
+    <t>Week 36</t>
+  </si>
+  <si>
+    <t>Week 37</t>
+  </si>
+  <si>
+    <t>Week 38</t>
+  </si>
+  <si>
+    <t>Daniel Burcham</t>
   </si>
 </sst>
 </file>
@@ -190,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -207,13 +225,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,11 +523,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH9"/>
+  <dimension ref="A1:AM10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE11" sqref="AE11"/>
+      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,9 +537,10 @@
     <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="20" width="9.140625" customWidth="1"/>
     <col min="21" max="21" width="9.140625" style="1"/>
+    <col min="36" max="36" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -613,8 +643,23 @@
       <c r="AH1" t="s">
         <v>41</v>
       </c>
+      <c r="AI1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -687,8 +732,17 @@
       <c r="AG2">
         <v>1.75</v>
       </c>
+      <c r="AI2">
+        <v>2.5</v>
+      </c>
+      <c r="AK2">
+        <v>3.5</v>
+      </c>
+      <c r="AM2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -738,7 +792,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -772,8 +826,11 @@
       <c r="AG4">
         <v>4</v>
       </c>
+      <c r="AL4">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -825,8 +882,17 @@
       <c r="AG5">
         <v>5.5</v>
       </c>
+      <c r="AI5">
+        <v>5</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK5">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -893,8 +959,20 @@
       <c r="AH6">
         <v>10</v>
       </c>
+      <c r="AJ6" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK6">
+        <v>6</v>
+      </c>
+      <c r="AL6">
+        <v>10</v>
+      </c>
+      <c r="AM6">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -949,8 +1027,17 @@
       <c r="AH7">
         <v>9</v>
       </c>
+      <c r="AI7">
+        <v>5.5</v>
+      </c>
+      <c r="AK7" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="AM7">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1011,8 +1098,17 @@
       <c r="AH8">
         <v>5</v>
       </c>
+      <c r="AJ8" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL8">
+        <v>3.5</v>
+      </c>
+      <c r="AM8">
+        <v>1.67</v>
+      </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1048,6 +1144,56 @@
       </c>
       <c r="AH9">
         <v>1.5</v>
+      </c>
+      <c r="AI9">
+        <v>1.5</v>
+      </c>
+      <c r="AJ9" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AM9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="1">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>5.5</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <v>7</v>
+      </c>
+      <c r="S10">
+        <v>7</v>
+      </c>
+      <c r="AK10">
+        <v>6.5</v>
+      </c>
+      <c r="AL10">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fall 22 week 7 InningCounts.xlsx
</commit_message>
<xml_diff>
--- a/data/InningCounts.xlsx
+++ b/data/InningCounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB020946-0370-47A6-9217-C15903D5DF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDE22B1-DE03-424B-AB1B-8A5CD7DB4130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="-30" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Player</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Week 41</t>
+  </si>
+  <si>
+    <t>Week 42</t>
   </si>
 </sst>
 </file>
@@ -531,11 +534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP10"/>
+  <dimension ref="A1:AQ10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP9" sqref="AP9"/>
+      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AN13" sqref="AN13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +551,7 @@
     <col min="36" max="36" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -675,8 +678,11 @@
       <c r="AP1" t="s">
         <v>50</v>
       </c>
+      <c r="AQ1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -764,8 +770,11 @@
       <c r="AO2">
         <v>10</v>
       </c>
+      <c r="AQ2">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -815,7 +824,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -861,8 +870,11 @@
       <c r="AP4">
         <v>5</v>
       </c>
+      <c r="AQ4">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -927,7 +939,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1009,8 +1021,11 @@
       <c r="AN6">
         <v>10</v>
       </c>
+      <c r="AQ6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1077,8 +1092,11 @@
       <c r="AO7">
         <v>5.5</v>
       </c>
+      <c r="AQ7">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1155,7 +1173,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1213,8 +1231,11 @@
       <c r="AP9">
         <v>1.5</v>
       </c>
+      <c r="AQ9">
+        <v>10</v>
+      </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
week 4 no match info entered this session
</commit_message>
<xml_diff>
--- a/data/InningCounts.xlsx
+++ b/data/InningCounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E2A4E0-8290-4E16-9D15-43041845C315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE944112-D75E-4500-9B17-46D73C22E07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2055" yWindow="1665" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Player</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Week 56</t>
+  </si>
+  <si>
+    <t>Week 57</t>
   </si>
 </sst>
 </file>
@@ -290,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -322,9 +325,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -632,11 +632,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BE10"/>
+  <dimension ref="A1:BF10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BE8" sqref="BE8"/>
+      <selection pane="topRight" activeCell="BF15" sqref="BF15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +683,7 @@
     <col min="56" max="56" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -855,8 +855,11 @@
       <c r="BE1" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="BF1" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -974,8 +977,11 @@
       <c r="BD2" s="10">
         <v>2.25</v>
       </c>
+      <c r="BF2">
+        <v>2.33</v>
+      </c>
     </row>
-    <row r="3" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1025,7 +1031,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1089,8 +1095,11 @@
       <c r="BC4" s="8">
         <v>10</v>
       </c>
+      <c r="BF4">
+        <v>5.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1175,11 +1184,11 @@
       <c r="BD5" s="8">
         <v>8</v>
       </c>
-      <c r="BE5" s="13">
+      <c r="BE5" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1292,7 +1301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1384,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -1478,8 +1487,11 @@
       <c r="BE8">
         <v>3</v>
       </c>
+      <c r="BF8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="9" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -1567,8 +1579,11 @@
       <c r="BE9">
         <v>3</v>
       </c>
+      <c r="BF9">
+        <v>1.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>

</xml_diff>